<commit_message>
Update 2025 entrants list
</commit_message>
<xml_diff>
--- a/resources/wip/entrants.xlsx
+++ b/resources/wip/entrants.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\mike\projects\work\wst-results\resources\wip\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64636576-05A4-457F-BAC6-D181561B62F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{365F6F56-2BB1-4BB9-9E22-453E38399DB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4B1638DB-7A97-4F10-A0EF-3AAE2DAC1F8E}"/>
+    <workbookView xWindow="-60" yWindow="-60" windowWidth="23160" windowHeight="13800" xr2:uid="{4B1638DB-7A97-4F10-A0EF-3AAE2DAC1F8E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="219">
   <si>
     <t>Harald Claessen                      </t>
   </si>
@@ -715,6 +715,9 @@
   </si>
   <si>
     <t>van der Hout            </t>
+  </si>
+  <si>
+    <t>FRA-95</t>
   </si>
 </sst>
 </file>
@@ -813,15 +816,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1156,28 +1157,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA21DFA1-AF3C-40D4-8DA2-86A18350D783}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:I51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="49.59765625" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.73046875" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.53125" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.3984375" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.19921875" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.19921875" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.86328125" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.19921875" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.06640625" style="4"/>
+    <col min="1" max="1" width="49.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>195</v>
       </c>
@@ -1206,7 +1208,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>29</v>
       </c>
@@ -1235,21 +1237,21 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="5"/>
-      <c r="C3" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="D3" s="5" t="s">
+      <c r="C3" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="3" t="s">
         <v>93</v>
       </c>
       <c r="G3" s="4" t="s">
@@ -1262,7 +1264,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>39</v>
       </c>
@@ -1291,7 +1293,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>44</v>
       </c>
@@ -1320,7 +1322,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>37</v>
       </c>
@@ -1349,7 +1351,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>45</v>
       </c>
@@ -1378,7 +1380,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
@@ -1407,8 +1409,8 @@
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A9" s="5" t="s">
+    <row r="9" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -1436,7 +1438,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>33</v>
       </c>
@@ -1465,7 +1467,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>28</v>
       </c>
@@ -1494,7 +1496,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>42</v>
       </c>
@@ -1523,7 +1525,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>20</v>
       </c>
@@ -1552,7 +1554,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>30</v>
       </c>
@@ -1581,7 +1583,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>46</v>
       </c>
@@ -1610,21 +1612,21 @@
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>27</v>
       </c>
       <c r="B16" s="5"/>
-      <c r="C16" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="D16" s="5" t="s">
+      <c r="C16" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D16" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="E16" s="5" t="s">
+      <c r="E16" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="F16" s="4" t="s">
+      <c r="F16" s="3" t="s">
         <v>93</v>
       </c>
       <c r="G16" s="4" t="s">
@@ -1637,21 +1639,21 @@
         <v>60</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>10</v>
       </c>
       <c r="B17" s="5"/>
-      <c r="C17" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="D17" s="5" t="s">
+      <c r="C17" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D17" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="E17" s="5" t="s">
+      <c r="E17" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="F17" s="4" t="s">
+      <c r="F17" s="3" t="s">
         <v>93</v>
       </c>
       <c r="G17" s="4" t="s">
@@ -1664,7 +1666,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>12</v>
       </c>
@@ -1693,7 +1695,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>32</v>
       </c>
@@ -1722,7 +1724,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>26</v>
       </c>
@@ -1751,21 +1753,21 @@
         <v>60</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B21" s="5"/>
-      <c r="C21" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="D21" s="5" t="s">
+      <c r="C21" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D21" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="E21" s="5" t="s">
+      <c r="E21" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="F21" s="4" t="s">
+      <c r="F21" s="3" t="s">
         <v>67</v>
       </c>
       <c r="G21" s="4" t="s">
@@ -1778,7 +1780,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>23</v>
       </c>
@@ -1807,7 +1809,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>0</v>
       </c>
@@ -1836,7 +1838,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>2</v>
       </c>
@@ -1865,7 +1867,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>41</v>
       </c>
@@ -1894,21 +1896,21 @@
         <v>60</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>18</v>
       </c>
       <c r="B26" s="5"/>
-      <c r="C26" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="D26" s="5" t="s">
+      <c r="C26" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D26" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="E26" s="5" t="s">
+      <c r="E26" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="F26" s="4" t="s">
+      <c r="F26" s="3" t="s">
         <v>209</v>
       </c>
       <c r="G26" s="4" t="s">
@@ -1921,34 +1923,36 @@
         <v>60</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A27" s="8" t="s">
+    <row r="27" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="7" t="s">
         <v>196</v>
       </c>
-      <c r="B27" s="6"/>
-      <c r="C27" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="D27" s="7" t="s">
+      <c r="B27" s="8" t="s">
+        <v>199</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="D27" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="E27" s="7" t="s">
+      <c r="E27" s="6" t="s">
         <v>184</v>
       </c>
-      <c r="F27" s="4" t="s">
+      <c r="F27" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="G27" s="4" t="s">
-        <v>200</v>
-      </c>
-      <c r="H27" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="I27" s="4" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="G27" s="8" t="s">
+        <v>218</v>
+      </c>
+      <c r="H27" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="I27" s="8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>15</v>
       </c>
@@ -1977,7 +1981,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="29" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>13</v>
       </c>
@@ -2006,7 +2010,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="30" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>36</v>
       </c>
@@ -2035,7 +2039,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="31" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>9</v>
       </c>
@@ -2064,11 +2068,11 @@
         <v>60</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A32" s="5" t="s">
+    <row r="32" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B32" s="5" t="s">
+      <c r="B32" s="2" t="s">
         <v>199</v>
       </c>
       <c r="C32" s="3" t="s">
@@ -2093,7 +2097,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
         <v>17</v>
       </c>
@@ -2120,34 +2124,34 @@
         <v>200</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A34" s="8" t="s">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="7" t="s">
         <v>197</v>
       </c>
-      <c r="B34" s="6"/>
-      <c r="C34" s="4" t="s">
+      <c r="B34" s="7"/>
+      <c r="C34" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="D34" s="7" t="s">
+      <c r="D34" s="6" t="s">
         <v>181</v>
       </c>
-      <c r="E34" s="7" t="s">
+      <c r="E34" s="6" t="s">
         <v>192</v>
       </c>
-      <c r="F34" s="4" t="s">
+      <c r="F34" s="8" t="s">
         <v>200</v>
       </c>
-      <c r="G34" s="4" t="s">
+      <c r="G34" s="8" t="s">
         <v>200</v>
       </c>
-      <c r="H34" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="I34" s="4" t="s">
+      <c r="H34" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="I34" s="8" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="35" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>34</v>
       </c>
@@ -2176,7 +2180,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="36" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>214</v>
       </c>
@@ -2205,7 +2209,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="37" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>43</v>
       </c>
@@ -2234,7 +2238,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="38" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>4</v>
       </c>
@@ -2263,21 +2267,21 @@
         <v>60</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
         <v>38</v>
       </c>
       <c r="B39" s="5"/>
-      <c r="C39" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="D39" s="5" t="s">
+      <c r="C39" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D39" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="E39" s="5" t="s">
+      <c r="E39" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="F39" s="4" t="s">
+      <c r="F39" s="3" t="s">
         <v>86</v>
       </c>
       <c r="G39" s="4" t="s">
@@ -2290,7 +2294,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="40" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>8</v>
       </c>
@@ -2319,7 +2323,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="41" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>24</v>
       </c>
@@ -2348,24 +2352,26 @@
         <v>60</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A42" s="5" t="s">
+    <row r="42" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B42" s="5"/>
-      <c r="C42" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="D42" s="5" t="s">
+      <c r="B42" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D42" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="E42" s="5" t="s">
+      <c r="E42" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="F42" s="4" t="s">
+      <c r="F42" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="G42" s="4" t="s">
+      <c r="G42" s="8" t="s">
         <v>215</v>
       </c>
       <c r="H42" s="3" t="s">
@@ -2375,7 +2381,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="43" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>14</v>
       </c>
@@ -2404,24 +2410,26 @@
         <v>60</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A44" s="5" t="s">
+    <row r="44" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B44" s="5"/>
-      <c r="C44" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="D44" s="5" t="s">
+      <c r="B44" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D44" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="E44" s="5" t="s">
+      <c r="E44" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="F44" s="4" t="s">
+      <c r="F44" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="G44" s="4" t="s">
+      <c r="G44" s="8" t="s">
         <v>213</v>
       </c>
       <c r="H44" s="3" t="s">
@@ -2431,7 +2439,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="45" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>3</v>
       </c>
@@ -2460,7 +2468,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="46" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>21</v>
       </c>
@@ -2489,24 +2497,26 @@
         <v>60</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A47" s="5" t="s">
+    <row r="47" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B47" s="5"/>
-      <c r="C47" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="D47" s="5" t="s">
+      <c r="B47" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D47" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="E47" s="5" t="s">
+      <c r="E47" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="F47" s="4" t="s">
+      <c r="F47" s="8" t="s">
         <v>209</v>
       </c>
-      <c r="G47" s="4" t="s">
+      <c r="G47" s="8" t="s">
         <v>210</v>
       </c>
       <c r="H47" s="3" t="s">
@@ -2516,21 +2526,21 @@
         <v>60</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B48" s="5"/>
-      <c r="C48" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="D48" s="5" t="s">
+      <c r="C48" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D48" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="E48" s="5" t="s">
+      <c r="E48" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="F48" s="4" t="s">
+      <c r="F48" s="3" t="s">
         <v>93</v>
       </c>
       <c r="G48" s="4" t="s">
@@ -2543,7 +2553,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="49" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>40</v>
       </c>
@@ -2572,7 +2582,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="50" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>19</v>
       </c>
@@ -2601,7 +2611,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="51" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>31</v>
       </c>
@@ -2631,7 +2641,11 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I51" xr:uid="{BA21DFA1-AF3C-40D4-8DA2-86A18350D783}"/>
+  <autoFilter ref="A1:I51" xr:uid="{BA21DFA1-AF3C-40D4-8DA2-86A18350D783}">
+    <filterColumn colId="1">
+      <filters blank="1"/>
+    </filterColumn>
+  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C2:I30">
     <sortCondition ref="D2:D30"/>
     <sortCondition ref="E2:E30"/>

</xml_diff>